<commit_message>
RETAKE gestionProd / ADD Idea_TowerDefense.docx
</commit_message>
<xml_diff>
--- a/Documents/_gestionProd/Roles.xlsx
+++ b/Documents/_gestionProd/Roles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GameSup_GD1\Workshop\Tower_Defense\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GameSup_GD1\Workshop\Tower_Defense\STD_Workshop\Documents\_gestionProd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CA818D-54B4-4ED3-86CE-859F982AA229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBF0E43-84D8-49FC-A77E-1D77FDC5F9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="360" windowWidth="21600" windowHeight="14040" xr2:uid="{43AE2A77-B1AA-4792-B95D-A9C147F61A7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43AE2A77-B1AA-4792-B95D-A9C147F61A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
     <t>Sculpting</t>
   </si>
   <si>
-    <t>Animations</t>
+    <t>/Animations/</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>